<commit_message>
DOC: Single-phase / thermochemical data fitting experiments
</commit_message>
<xml_diff>
--- a/research/almg_test_thermochemical.xlsx
+++ b/research/almg_test_thermochemical.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="11">
   <si>
     <t>T</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>MIX_HM</t>
+  </si>
+  <si>
+    <t>P</t>
   </si>
 </sst>
 </file>
@@ -378,18 +381,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -397,19 +400,22 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -417,20 +423,23 @@
         <v>1080</v>
       </c>
       <c r="C2">
-        <f>1-D2</f>
+        <v>101325</v>
+      </c>
+      <c r="D2">
+        <f>1-E2</f>
         <v>0.19999999999999996</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>0.8</v>
       </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="1">
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="1">
         <v>-1400</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -438,20 +447,23 @@
         <v>1080</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C11" si="0">1-D3</f>
+        <v>101325</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D11" si="0">1-E3</f>
         <v>0.4</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>0.6</v>
       </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="1">
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="1">
         <v>-2050</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -459,20 +471,23 @@
         <v>1080</v>
       </c>
       <c r="C4">
+        <v>101325</v>
+      </c>
+      <c r="D4">
         <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>0.4</v>
       </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="1">
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="1">
         <v>-2200</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -480,20 +495,23 @@
         <v>1080</v>
       </c>
       <c r="C5">
+        <v>101325</v>
+      </c>
+      <c r="D5">
         <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>0.2</v>
       </c>
-      <c r="E5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="1">
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="1">
         <v>-1600</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -501,20 +519,23 @@
         <v>298.14999999999998</v>
       </c>
       <c r="C6">
+        <v>101325</v>
+      </c>
+      <c r="D6">
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>0.25</v>
       </c>
-      <c r="E6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="1">
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="1">
         <v>525</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -522,20 +543,23 @@
         <v>298.14999999999998</v>
       </c>
       <c r="C7">
+        <v>101325</v>
+      </c>
+      <c r="D7">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>0.5</v>
       </c>
-      <c r="E7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="1">
+      <c r="F7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="1">
         <v>1174</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -543,20 +567,23 @@
         <v>298.14999999999998</v>
       </c>
       <c r="C8">
+        <v>101325</v>
+      </c>
+      <c r="D8">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>0.75</v>
       </c>
-      <c r="E8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="1">
+      <c r="F8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="1">
         <v>852</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -564,20 +591,23 @@
         <v>298.14999999999998</v>
       </c>
       <c r="C9">
+        <v>101325</v>
+      </c>
+      <c r="D9">
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>0.25</v>
       </c>
-      <c r="E9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="1">
+      <c r="F9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="1">
         <v>372</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -585,20 +615,23 @@
         <v>298.14999999999998</v>
       </c>
       <c r="C10">
+        <v>101325</v>
+      </c>
+      <c r="D10">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>0.5</v>
       </c>
-      <c r="E10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="1">
+      <c r="F10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="1">
         <v>394</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -606,16 +639,19 @@
         <v>298.14999999999998</v>
       </c>
       <c r="C11">
+        <v>101325</v>
+      </c>
+      <c r="D11">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>0.75</v>
       </c>
-      <c r="E11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="1">
+      <c r="F11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="1">
         <v>146</v>
       </c>
     </row>

</xml_diff>